<commit_message>
added general cost equations
</commit_message>
<xml_diff>
--- a/IPSF Cost Effectiveness Model.xlsx
+++ b/IPSF Cost Effectiveness Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dnz-my.sharepoint.com/personal/ben_marmont_dairynz_co_nz/Documents/Documents/Thesis/Economic Modelling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dnz-my.sharepoint.com/personal/ben_marmont_dairynz_co_nz/Documents/Documents/R/Public Masters Repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4212" documentId="8_{F0DCD7A2-AC69-4F97-85AC-5004E407EC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{019A4C17-0F70-497A-BF2E-549CA25380B1}"/>
+  <xr:revisionPtr revIDLastSave="4451" documentId="8_{F0DCD7A2-AC69-4F97-85AC-5004E407EC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6C1B4EE-0619-418C-8995-1269F3A5A15B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15930" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="10" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="444">
   <si>
     <t>Assumptions</t>
   </si>
@@ -1148,12 +1148,6 @@
     <t>Total Supplement (t/cow/pa)</t>
   </si>
   <si>
-    <t>Incumbent Quantity (kg/cow/day)</t>
-  </si>
-  <si>
-    <t>Premium Quantity (kg/cow/day)</t>
-  </si>
-  <si>
     <t>Incumbent Price ($/t)</t>
   </si>
   <si>
@@ -1167,12 +1161,6 @@
   </si>
   <si>
     <t>Total imported feed</t>
-  </si>
-  <si>
-    <t>Incumbent (t/cow/year)</t>
-  </si>
-  <si>
-    <t>Premium (t/cow/year)</t>
   </si>
   <si>
     <t>Value Imported feed</t>
@@ -1364,6 +1352,329 @@
   </si>
   <si>
     <t>The 'sib models' sheet contains the scaling of costs and revenue associated with the approach.</t>
+  </si>
+  <si>
+    <t>General Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cost of 3NOP </t>
+  </si>
+  <si>
+    <t>Per cow cost of 3NOP</t>
+  </si>
+  <si>
+    <t>Total cost of Asparagopsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of Asparagopsis * AUD:NZD * Dietary Inclusion Rate * Yearly DMI </t>
+  </si>
+  <si>
+    <t>Per cow cost of Asparagopsis</t>
+  </si>
+  <si>
+    <t>General Form Equation</t>
+  </si>
+  <si>
+    <t>Marginal cost of supplement cow/year</t>
+  </si>
+  <si>
+    <r>
+      <t>Premium Quantity (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/cow/day)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Incumbent Quantity (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/cow/day)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Incumbent (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/cow/year)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Premium (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/cow/year)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost of 3NOP* Euro:NZD * 11.5 * milksolid production per cow </t>
+  </si>
+  <si>
+    <t>Cost of 3NOP* Euro:NZD * 11.5 * total farm milksolid production * implementation period</t>
+  </si>
+  <si>
+    <t>Cost of Asparagopsis * AUD:NZD * Dietary Inclusion Rate * Yearly DMI * Herd size * implementation period</t>
+  </si>
+  <si>
+    <t>[(daily premium allocation * $premium *365/1000)-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(daily incumbent allocation * $incumbent * 365/1000)] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* implementation preiod </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine count = round up to whole number, Herd size / 200 </t>
+  </si>
+  <si>
+    <t>machine count * monthly maintenance +</t>
+  </si>
+  <si>
+    <t>* implementation period</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> machine count * monthly rental +  </t>
+  </si>
+  <si>
+    <t>Labour cost =</t>
+  </si>
+  <si>
+    <t>weekly time * 52 / 2400 * $FTE * machine count</t>
+  </si>
+  <si>
+    <t>Methane emissions (kg) = DMI(kg) * emissions factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abated emissions % = </t>
+  </si>
+  <si>
+    <t>[dry cow count * dry DMI * days as dry cow * dry cow emission factor * (1-assumed mitigation)]</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>[milking cow count * DMI * days as milker * milker emission factor * (1-assumed mitigation)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum for stock classes [stock class cow count * stock class DMI * days in stock class * </t>
+  </si>
+  <si>
+    <t>stock class emissions factor *assumed mitigation * % delivery period for stock class]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of additional milk production = </t>
+  </si>
+  <si>
+    <t>assumed 85 DM%</t>
+  </si>
+  <si>
+    <t>assumed MS response coefficient of 55g/MS kg DM</t>
+  </si>
+  <si>
+    <t>additional supplement(kg/cow/pa) * DM% of supplement * MS response coefficient * milk payout * herd size</t>
+  </si>
+  <si>
+    <t>Equations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Smart Feeder Count =   Herd size / 200 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(round up to whole number)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine cost = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macine cost = (machine count * monthly rental + machine count * monthly maintenance) * implementation period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smart Feeder Machine Cost = (machine count * monthly rental + machine count * monthly maintenance) * implementation period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(daily premium allocation * $premium *365/1000) - (daily incumbent allocation * $incumbent * 365/1000)] * implementation preiod </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Supplementary Feed Cost = [(daily premium allocation * $premium *365/1000) - (daily incumbent allocation * $incumbent * 365/1000)] * implementation preiod </t>
+  </si>
+  <si>
+    <r>
+      <t>Milk Response to Additional Supplement = additional supplement</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(kg/cow/pa)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * DM% of supplement * MS response coefficient * milk payout * herd size</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Smart Feeder Labour Cost = hours(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>machine/week)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * 52 / 2400 * $FTE * machine count</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Methane Inhibitor Cost (3NOP) = Cost of 3NOP * Euro:NZD * 11.5 * total farm milksolid production * implementation period</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Methane Mitigation (Abated) = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sum for stock classes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [stock class cow count * stock class DMI * days in stock class * stock class emissions factor *assumed mitigation * % delivery period for stock class]</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Methane Inhibitor Cost (Asparagopsis) = Cost of Asparagopsis * AUD:NZD * Dietary Inclusion Rate * Yearly DMI * implementation period</t>
   </si>
 </sst>
 </file>
@@ -1929,7 +2240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2114,11 +2425,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2130,6 +2437,8 @@
     <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2178,18 +2487,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2206,10 +2527,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2551,12 +2868,12 @@
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="98" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="98" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2606,17 +2923,17 @@
     </row>
     <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="98" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="98" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="98" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4089,7 +4406,7 @@
   </sheetPr>
   <dimension ref="C3:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -4105,14 +4422,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="99" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E4" s="99"/>
     </row>
     <row r="5" spans="3:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C5" s="99"/>
       <c r="D5" s="99" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E5" s="99"/>
     </row>
@@ -4121,7 +4438,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E6" s="99"/>
     </row>
@@ -4157,7 +4474,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="99" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="31.5" x14ac:dyDescent="0.5">
@@ -4167,23 +4484,23 @@
     </row>
     <row r="17" spans="4:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D17" s="99" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E17" s="95"/>
     </row>
     <row r="18" spans="4:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D18" s="99" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D19" s="99" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D20" s="99" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -4199,7 +4516,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4209,8 +4526,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="183" t="s">
-        <v>360</v>
+      <c r="A1" s="153" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4254,8 +4571,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="183" t="s">
-        <v>361</v>
+      <c r="A8" s="153" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4263,7 +4580,7 @@
         <v>50</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,7 +4588,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="131">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4299,12 +4616,12 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B14" s="132" t="s">
         <v>41</v>
@@ -4315,7 +4632,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="57">
-        <v>1</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4343,8 +4660,8 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="183" t="s">
-        <v>362</v>
+      <c r="A20" s="153" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4352,12 +4669,12 @@
         <v>93</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B22" s="57">
         <v>30</v>
@@ -4421,7 +4738,7 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A2:E72"/>
+  <dimension ref="B2:D71"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
@@ -4435,21 +4752,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="154" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
+      <c r="B3" s="155"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
     </row>
     <row r="4" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="157"/>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
+      <c r="B4" s="155"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
     </row>
     <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="108" t="str">
@@ -4682,7 +4999,7 @@
       </c>
       <c r="D23" s="92">
         <f>Financials!P18</f>
-        <v>239967.5512523081</v>
+        <v>228807.5512523081</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -4752,7 +5069,7 @@
       </c>
       <c r="D28" s="106">
         <f>Financials!P23</f>
-        <v>659348.64337047166</v>
+        <v>648188.64337047166</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -4804,7 +5121,7 @@
       </c>
       <c r="D34" s="106">
         <f>Financials!P27</f>
-        <v>252238.99870427116</v>
+        <v>263398.99870427116</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -4844,7 +5161,7 @@
       </c>
       <c r="D38" s="91">
         <f>Financials!P31</f>
-        <v>772968.21544015384</v>
+        <v>761808.21544015384</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -4858,7 +5175,7 @@
       </c>
       <c r="D39" s="92">
         <f>Financials!P32</f>
-        <v>138619.42663458898</v>
+        <v>149779.42663458898</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4872,7 +5189,7 @@
       </c>
       <c r="D40" s="107">
         <f>Financials!P33</f>
-        <v>0.15206374048588003</v>
+        <v>0.1643061179435211</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -4926,7 +5243,7 @@
       </c>
       <c r="D45" s="112">
         <f>Financials!P38-D61</f>
-        <v>99447.393835616414</v>
+        <v>106547.94383561642</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -4940,7 +5257,7 @@
       </c>
       <c r="D46" s="114">
         <f>D45/D44</f>
-        <v>11.001304685563124</v>
+        <v>11.786798512723617</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4954,103 +5271,103 @@
       </c>
       <c r="D47" s="117">
         <f>D46/28*1000</f>
-        <v>392.9037387701116</v>
+        <v>420.95708974012916</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="30"/>
       <c r="D48" s="29"/>
     </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B49" s="146" t="str">
+    <row r="49" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B49" s="142" t="str">
         <f>Financials!N42</f>
         <v>Operating Cash and Non-cash (With Emission Pricing)</v>
       </c>
-      <c r="C49" s="147" t="str">
+      <c r="C49" s="143" t="str">
         <f>Financials!O42</f>
         <v>Baseline</v>
       </c>
-      <c r="D49" s="148" t="str">
+      <c r="D49" s="144" t="str">
         <f>Financials!P42</f>
         <v>Adopter</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="145" t="str">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="141" t="str">
         <f>Financials!N43</f>
         <v>Dairy Gross Farm Revenue</v>
       </c>
-      <c r="C50" s="149">
+      <c r="C50" s="145">
         <f>Financials!O43</f>
         <v>911587.64207474282</v>
       </c>
-      <c r="D50" s="150">
+      <c r="D50" s="146">
         <f>Financials!P43</f>
         <v>911587.64207474282</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="145" t="str">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="141" t="str">
         <f>Financials!N44</f>
         <v>Dairy Operating Expense</v>
       </c>
-      <c r="C51" s="149">
+      <c r="C51" s="145">
         <f>Financials!O44</f>
         <v>643086.57160453743</v>
       </c>
-      <c r="D51" s="150">
+      <c r="D51" s="146">
         <f>Financials!P44</f>
-        <v>772968.21544015384</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="151" t="str">
+        <v>761808.21544015384</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="147" t="str">
         <f>Financials!N45</f>
         <v>Emission Charge</v>
       </c>
-      <c r="C52" s="152">
+      <c r="C52" s="148">
         <f>Financials!O45</f>
-        <v>476713.73718924396</v>
-      </c>
-      <c r="D52" s="153">
+        <v>435752.40385591058</v>
+      </c>
+      <c r="D52" s="149">
         <f>Financials!P45</f>
-        <v>346832.09335362754</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="145" t="str">
+        <v>317030.76002029423</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="141" t="str">
         <f>Financials!N46</f>
         <v>Dairy Operating Profit</v>
       </c>
-      <c r="C53" s="149">
+      <c r="C53" s="145">
         <f>Financials!O46</f>
-        <v>-208212.66671903856</v>
-      </c>
-      <c r="D53" s="150">
+        <v>-167251.33338570519</v>
+      </c>
+      <c r="D53" s="146">
         <f>Financials!P46</f>
-        <v>-208212.66671903856</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="145" t="str">
+        <v>-167251.33338570525</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="141" t="str">
         <f>Financials!N47</f>
         <v>Dairy Profit Margin</v>
       </c>
-      <c r="C54" s="154">
+      <c r="C54" s="150">
         <f>Financials!O47</f>
-        <v>-0.22840663597101155</v>
-      </c>
-      <c r="D54" s="155">
+        <v>-0.18347257648759563</v>
+      </c>
+      <c r="D54" s="151">
         <f>Financials!P47</f>
-        <v>-0.22840663597101155</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-0.18347257648759568</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="28"/>
       <c r="C55" s="128"/>
       <c r="D55" s="129"/>
     </row>
-    <row r="56" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B56" s="108" t="str">
         <f>Financials!N49</f>
         <v>Feed Composition</v>
@@ -5064,49 +5381,49 @@
         <v>Adopter</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="30" t="str">
         <f>Financials!N50</f>
         <v>Total Imported Feed (t/year)</v>
       </c>
       <c r="C57">
         <f>Financials!O50</f>
-        <v>0</v>
+        <v>135.78</v>
       </c>
       <c r="D57" s="29">
         <f>Financials!P50</f>
-        <v>113.14999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>181.04</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="82" t="str">
         <f>Financials!N51</f>
         <v>Cost of Imported Feed ($/year)</v>
       </c>
       <c r="C58" s="48">
         <f>Financials!O51</f>
-        <v>0</v>
+        <v>67890</v>
       </c>
       <c r="D58" s="91">
         <f>Financials!P51</f>
-        <v>90520</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144832</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="30" t="str">
         <f>Financials!N52</f>
         <v>Pasture Proportion of Diet (relative to premium supplement)</v>
       </c>
       <c r="C59" s="26">
         <f>Financials!O52</f>
-        <v>1</v>
+        <v>0.92486377396569119</v>
       </c>
       <c r="D59" s="89">
         <f>Financials!P52</f>
-        <v>0.93738647830474264</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.89981836528758841</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="82" t="str">
         <f>Financials!N53</f>
         <v>Pasture Uitilisation Forgone</v>
@@ -5117,12 +5434,12 @@
       </c>
       <c r="D60" s="93">
         <f>Financials!P53</f>
-        <v>6.2613521695257357E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.5045408678102787E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="54" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C61" s="138" t="str">
         <f>"-"</f>
@@ -5130,78 +5447,32 @@
       </c>
       <c r="D61" s="112">
         <f>'sub-models'!AN29</f>
-        <v>30434.25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="172"/>
-      <c r="B63" s="172"/>
-      <c r="C63" s="172"/>
-      <c r="D63" s="172"/>
-      <c r="E63" s="172"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="172"/>
-      <c r="B64" s="173"/>
-      <c r="C64" s="172"/>
-      <c r="D64" s="172"/>
-      <c r="E64" s="172"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="172"/>
-      <c r="B65" s="172"/>
-      <c r="C65" s="174"/>
-      <c r="D65" s="172"/>
-      <c r="E65" s="172"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="172"/>
-      <c r="B66" s="172"/>
-      <c r="C66" s="174"/>
-      <c r="D66" s="172"/>
-      <c r="E66" s="172"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="172"/>
-      <c r="B67" s="172"/>
-      <c r="C67" s="174"/>
-      <c r="D67" s="172"/>
-      <c r="E67" s="172"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="172"/>
-      <c r="B68" s="172"/>
-      <c r="C68" s="175"/>
-      <c r="D68" s="172"/>
-      <c r="E68" s="172"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="172"/>
-      <c r="B69" s="172"/>
-      <c r="C69" s="176"/>
-      <c r="D69" s="172"/>
-      <c r="E69" s="172"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="172"/>
-      <c r="B70" s="172"/>
-      <c r="C70" s="174"/>
-      <c r="D70" s="172"/>
-      <c r="E70" s="172"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="172"/>
-      <c r="B71" s="172"/>
-      <c r="C71" s="175"/>
-      <c r="D71" s="172"/>
-      <c r="E71" s="172"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="172"/>
-      <c r="B72" s="172"/>
-      <c r="C72" s="172"/>
-      <c r="D72" s="172"/>
-      <c r="E72" s="172"/>
+        <v>12173.700000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="47"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="47"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="47"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="75"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="25"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="47"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5217,8 +5488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5450D72-D253-4275-AC22-02640FB77BAE}">
   <dimension ref="A1:AC48"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5267,15 +5538,15 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="158" t="s">
+      <c r="K2" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="158"/>
-      <c r="N2" s="158" t="s">
+      <c r="L2" s="156"/>
+      <c r="N2" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="156"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5455,7 +5726,7 @@
         <v>46</v>
       </c>
       <c r="N8" s="69" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="O8" s="22">
         <f>0</f>
@@ -5480,32 +5751,32 @@
       <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="159" t="s">
-        <v>365</v>
-      </c>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="159"/>
-      <c r="U9" s="159"/>
-      <c r="V9" s="159"/>
-      <c r="W9" s="159"/>
-      <c r="X9" s="159"/>
-      <c r="Y9" s="159"/>
-      <c r="Z9" s="159"/>
-      <c r="AA9" s="159"/>
-      <c r="AB9" s="159"/>
-      <c r="AC9" s="159"/>
+      <c r="F9" s="157" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="157"/>
+      <c r="K9" s="157"/>
+      <c r="L9" s="157"/>
+      <c r="M9" s="157"/>
+      <c r="N9" s="157"/>
+      <c r="O9" s="157"/>
+      <c r="P9" s="157"/>
+      <c r="Q9" s="157"/>
+      <c r="R9" s="157"/>
+      <c r="S9" s="157"/>
+      <c r="T9" s="157"/>
+      <c r="U9" s="157"/>
+      <c r="V9" s="157"/>
+      <c r="W9" s="157"/>
+      <c r="X9" s="157"/>
+      <c r="Y9" s="157"/>
+      <c r="Z9" s="157"/>
+      <c r="AA9" s="157"/>
+      <c r="AB9" s="157"/>
+      <c r="AC9" s="157"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5522,30 +5793,30 @@
       <c r="E10" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
-      <c r="N10" s="159"/>
-      <c r="O10" s="159"/>
-      <c r="P10" s="159"/>
-      <c r="Q10" s="159"/>
-      <c r="R10" s="159"/>
-      <c r="S10" s="159"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="159"/>
-      <c r="X10" s="159"/>
-      <c r="Y10" s="159"/>
-      <c r="Z10" s="159"/>
-      <c r="AA10" s="159"/>
-      <c r="AB10" s="159"/>
-      <c r="AC10" s="159"/>
+      <c r="F10" s="157"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="157"/>
+      <c r="K10" s="157"/>
+      <c r="L10" s="157"/>
+      <c r="M10" s="157"/>
+      <c r="N10" s="157"/>
+      <c r="O10" s="157"/>
+      <c r="P10" s="157"/>
+      <c r="Q10" s="157"/>
+      <c r="R10" s="157"/>
+      <c r="S10" s="157"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
+      <c r="V10" s="157"/>
+      <c r="W10" s="157"/>
+      <c r="X10" s="157"/>
+      <c r="Y10" s="157"/>
+      <c r="Z10" s="157"/>
+      <c r="AA10" s="157"/>
+      <c r="AB10" s="157"/>
+      <c r="AC10" s="157"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -5553,39 +5824,39 @@
       </c>
       <c r="B11" s="3">
         <f>Inputs!B10</f>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C11" s="3">
         <f>B11</f>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="159"/>
-      <c r="L11" s="159"/>
-      <c r="M11" s="159"/>
-      <c r="N11" s="159"/>
-      <c r="O11" s="159"/>
-      <c r="P11" s="159"/>
-      <c r="Q11" s="159"/>
-      <c r="R11" s="159"/>
-      <c r="S11" s="159"/>
-      <c r="T11" s="159"/>
-      <c r="U11" s="159"/>
-      <c r="V11" s="159"/>
-      <c r="W11" s="159"/>
-      <c r="X11" s="159"/>
-      <c r="Y11" s="159"/>
-      <c r="Z11" s="159"/>
-      <c r="AA11" s="159"/>
-      <c r="AB11" s="159"/>
-      <c r="AC11" s="159"/>
+      <c r="F11" s="157"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="157"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
+      <c r="K11" s="157"/>
+      <c r="L11" s="157"/>
+      <c r="M11" s="157"/>
+      <c r="N11" s="157"/>
+      <c r="O11" s="157"/>
+      <c r="P11" s="157"/>
+      <c r="Q11" s="157"/>
+      <c r="R11" s="157"/>
+      <c r="S11" s="157"/>
+      <c r="T11" s="157"/>
+      <c r="U11" s="157"/>
+      <c r="V11" s="157"/>
+      <c r="W11" s="157"/>
+      <c r="X11" s="157"/>
+      <c r="Y11" s="157"/>
+      <c r="Z11" s="157"/>
+      <c r="AA11" s="157"/>
+      <c r="AB11" s="157"/>
+      <c r="AC11" s="157"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -5602,30 +5873,30 @@
       <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="159"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="159"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
-      <c r="K12" s="159"/>
-      <c r="L12" s="159"/>
-      <c r="M12" s="159"/>
-      <c r="N12" s="159"/>
-      <c r="O12" s="159"/>
-      <c r="P12" s="159"/>
-      <c r="Q12" s="159"/>
-      <c r="R12" s="159"/>
-      <c r="S12" s="159"/>
-      <c r="T12" s="159"/>
-      <c r="U12" s="159"/>
-      <c r="V12" s="159"/>
-      <c r="W12" s="159"/>
-      <c r="X12" s="159"/>
-      <c r="Y12" s="159"/>
-      <c r="Z12" s="159"/>
-      <c r="AA12" s="159"/>
-      <c r="AB12" s="159"/>
-      <c r="AC12" s="159"/>
+      <c r="F12" s="157"/>
+      <c r="G12" s="157"/>
+      <c r="H12" s="157"/>
+      <c r="I12" s="157"/>
+      <c r="J12" s="157"/>
+      <c r="K12" s="157"/>
+      <c r="L12" s="157"/>
+      <c r="M12" s="157"/>
+      <c r="N12" s="157"/>
+      <c r="O12" s="157"/>
+      <c r="P12" s="157"/>
+      <c r="Q12" s="157"/>
+      <c r="R12" s="157"/>
+      <c r="S12" s="157"/>
+      <c r="T12" s="157"/>
+      <c r="U12" s="157"/>
+      <c r="V12" s="157"/>
+      <c r="W12" s="157"/>
+      <c r="X12" s="157"/>
+      <c r="Y12" s="157"/>
+      <c r="Z12" s="157"/>
+      <c r="AA12" s="157"/>
+      <c r="AB12" s="157"/>
+      <c r="AC12" s="157"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -5642,30 +5913,30 @@
       <c r="E13" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
-      <c r="L13" s="159"/>
-      <c r="M13" s="159"/>
-      <c r="N13" s="159"/>
-      <c r="O13" s="159"/>
-      <c r="P13" s="159"/>
-      <c r="Q13" s="159"/>
-      <c r="R13" s="159"/>
-      <c r="S13" s="159"/>
-      <c r="T13" s="159"/>
-      <c r="U13" s="159"/>
-      <c r="V13" s="159"/>
-      <c r="W13" s="159"/>
-      <c r="X13" s="159"/>
-      <c r="Y13" s="159"/>
-      <c r="Z13" s="159"/>
-      <c r="AA13" s="159"/>
-      <c r="AB13" s="159"/>
-      <c r="AC13" s="159"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="157"/>
+      <c r="L13" s="157"/>
+      <c r="M13" s="157"/>
+      <c r="N13" s="157"/>
+      <c r="O13" s="157"/>
+      <c r="P13" s="157"/>
+      <c r="Q13" s="157"/>
+      <c r="R13" s="157"/>
+      <c r="S13" s="157"/>
+      <c r="T13" s="157"/>
+      <c r="U13" s="157"/>
+      <c r="V13" s="157"/>
+      <c r="W13" s="157"/>
+      <c r="X13" s="157"/>
+      <c r="Y13" s="157"/>
+      <c r="Z13" s="157"/>
+      <c r="AA13" s="157"/>
+      <c r="AB13" s="157"/>
+      <c r="AC13" s="157"/>
     </row>
     <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -5682,30 +5953,30 @@
       <c r="E14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
-      <c r="L14" s="159"/>
-      <c r="M14" s="159"/>
-      <c r="N14" s="159"/>
-      <c r="O14" s="159"/>
-      <c r="P14" s="159"/>
-      <c r="Q14" s="159"/>
-      <c r="R14" s="159"/>
-      <c r="S14" s="159"/>
-      <c r="T14" s="159"/>
-      <c r="U14" s="159"/>
-      <c r="V14" s="159"/>
-      <c r="W14" s="159"/>
-      <c r="X14" s="159"/>
-      <c r="Y14" s="159"/>
-      <c r="Z14" s="159"/>
-      <c r="AA14" s="159"/>
-      <c r="AB14" s="159"/>
-      <c r="AC14" s="159"/>
+      <c r="F14" s="157"/>
+      <c r="G14" s="157"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="157"/>
+      <c r="K14" s="157"/>
+      <c r="L14" s="157"/>
+      <c r="M14" s="157"/>
+      <c r="N14" s="157"/>
+      <c r="O14" s="157"/>
+      <c r="P14" s="157"/>
+      <c r="Q14" s="157"/>
+      <c r="R14" s="157"/>
+      <c r="S14" s="157"/>
+      <c r="T14" s="157"/>
+      <c r="U14" s="157"/>
+      <c r="V14" s="157"/>
+      <c r="W14" s="157"/>
+      <c r="X14" s="157"/>
+      <c r="Y14" s="157"/>
+      <c r="Z14" s="157"/>
+      <c r="AA14" s="157"/>
+      <c r="AB14" s="157"/>
+      <c r="AC14" s="157"/>
     </row>
     <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -5715,37 +5986,37 @@
         <f>Inputs!B14</f>
         <v>All Season</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="179">
         <f>VLOOKUP(B15,N3:P8,2,FALSE)</f>
         <v>0.82191780821917804</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
-      <c r="L15" s="159"/>
-      <c r="M15" s="159"/>
-      <c r="N15" s="159"/>
-      <c r="O15" s="159"/>
-      <c r="P15" s="159"/>
-      <c r="Q15" s="159"/>
-      <c r="R15" s="159"/>
-      <c r="S15" s="159"/>
-      <c r="T15" s="159"/>
-      <c r="U15" s="159"/>
-      <c r="V15" s="159"/>
-      <c r="W15" s="159"/>
-      <c r="X15" s="159"/>
-      <c r="Y15" s="159"/>
-      <c r="Z15" s="159"/>
-      <c r="AA15" s="159"/>
-      <c r="AB15" s="159"/>
-      <c r="AC15" s="159"/>
+      <c r="F15" s="157"/>
+      <c r="G15" s="157"/>
+      <c r="H15" s="157"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="157"/>
+      <c r="K15" s="157"/>
+      <c r="L15" s="157"/>
+      <c r="M15" s="157"/>
+      <c r="N15" s="157"/>
+      <c r="O15" s="157"/>
+      <c r="P15" s="157"/>
+      <c r="Q15" s="157"/>
+      <c r="R15" s="157"/>
+      <c r="S15" s="157"/>
+      <c r="T15" s="157"/>
+      <c r="U15" s="157"/>
+      <c r="V15" s="157"/>
+      <c r="W15" s="157"/>
+      <c r="X15" s="157"/>
+      <c r="Y15" s="157"/>
+      <c r="Z15" s="157"/>
+      <c r="AA15" s="157"/>
+      <c r="AB15" s="157"/>
+      <c r="AC15" s="157"/>
     </row>
     <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -5758,30 +6029,30 @@
       <c r="E16" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
-      <c r="M16" s="159"/>
-      <c r="N16" s="159"/>
-      <c r="O16" s="159"/>
-      <c r="P16" s="159"/>
-      <c r="Q16" s="159"/>
-      <c r="R16" s="159"/>
-      <c r="S16" s="159"/>
-      <c r="T16" s="159"/>
-      <c r="U16" s="159"/>
-      <c r="V16" s="159"/>
-      <c r="W16" s="159"/>
-      <c r="X16" s="159"/>
-      <c r="Y16" s="159"/>
-      <c r="Z16" s="159"/>
-      <c r="AA16" s="159"/>
-      <c r="AB16" s="159"/>
-      <c r="AC16" s="159"/>
+      <c r="F16" s="157"/>
+      <c r="G16" s="157"/>
+      <c r="H16" s="157"/>
+      <c r="I16" s="157"/>
+      <c r="J16" s="157"/>
+      <c r="K16" s="157"/>
+      <c r="L16" s="157"/>
+      <c r="M16" s="157"/>
+      <c r="N16" s="157"/>
+      <c r="O16" s="157"/>
+      <c r="P16" s="157"/>
+      <c r="Q16" s="157"/>
+      <c r="R16" s="157"/>
+      <c r="S16" s="157"/>
+      <c r="T16" s="157"/>
+      <c r="U16" s="157"/>
+      <c r="V16" s="157"/>
+      <c r="W16" s="157"/>
+      <c r="X16" s="157"/>
+      <c r="Y16" s="157"/>
+      <c r="Z16" s="157"/>
+      <c r="AA16" s="157"/>
+      <c r="AB16" s="157"/>
+      <c r="AC16" s="157"/>
     </row>
     <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -5801,82 +6072,82 @@
       <c r="E17" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
-      <c r="L17" s="159"/>
-      <c r="M17" s="159"/>
-      <c r="N17" s="159"/>
-      <c r="O17" s="159"/>
-      <c r="P17" s="159"/>
-      <c r="Q17" s="159"/>
-      <c r="R17" s="159"/>
-      <c r="S17" s="159"/>
-      <c r="T17" s="159"/>
-      <c r="U17" s="159"/>
-      <c r="V17" s="159"/>
-      <c r="W17" s="159"/>
-      <c r="X17" s="159"/>
-      <c r="Y17" s="159"/>
-      <c r="Z17" s="159"/>
-      <c r="AA17" s="159"/>
-      <c r="AB17" s="159"/>
-      <c r="AC17" s="159"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="157"/>
+      <c r="H17" s="157"/>
+      <c r="I17" s="157"/>
+      <c r="J17" s="157"/>
+      <c r="K17" s="157"/>
+      <c r="L17" s="157"/>
+      <c r="M17" s="157"/>
+      <c r="N17" s="157"/>
+      <c r="O17" s="157"/>
+      <c r="P17" s="157"/>
+      <c r="Q17" s="157"/>
+      <c r="R17" s="157"/>
+      <c r="S17" s="157"/>
+      <c r="T17" s="157"/>
+      <c r="U17" s="157"/>
+      <c r="V17" s="157"/>
+      <c r="W17" s="157"/>
+      <c r="X17" s="157"/>
+      <c r="Y17" s="157"/>
+      <c r="Z17" s="157"/>
+      <c r="AA17" s="157"/>
+      <c r="AB17" s="157"/>
+      <c r="AC17" s="157"/>
     </row>
     <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
-      <c r="L18" s="159"/>
-      <c r="M18" s="159"/>
-      <c r="N18" s="159"/>
-      <c r="O18" s="159"/>
-      <c r="P18" s="159"/>
-      <c r="Q18" s="159"/>
-      <c r="R18" s="159"/>
-      <c r="S18" s="159"/>
-      <c r="T18" s="159"/>
-      <c r="U18" s="159"/>
-      <c r="V18" s="159"/>
-      <c r="W18" s="159"/>
-      <c r="X18" s="159"/>
-      <c r="Y18" s="159"/>
-      <c r="Z18" s="159"/>
-      <c r="AA18" s="159"/>
-      <c r="AB18" s="159"/>
-      <c r="AC18" s="159"/>
+      <c r="F18" s="157"/>
+      <c r="G18" s="157"/>
+      <c r="H18" s="157"/>
+      <c r="I18" s="157"/>
+      <c r="J18" s="157"/>
+      <c r="K18" s="157"/>
+      <c r="L18" s="157"/>
+      <c r="M18" s="157"/>
+      <c r="N18" s="157"/>
+      <c r="O18" s="157"/>
+      <c r="P18" s="157"/>
+      <c r="Q18" s="157"/>
+      <c r="R18" s="157"/>
+      <c r="S18" s="157"/>
+      <c r="T18" s="157"/>
+      <c r="U18" s="157"/>
+      <c r="V18" s="157"/>
+      <c r="W18" s="157"/>
+      <c r="X18" s="157"/>
+      <c r="Y18" s="157"/>
+      <c r="Z18" s="157"/>
+      <c r="AA18" s="157"/>
+      <c r="AB18" s="157"/>
+      <c r="AC18" s="157"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="159"/>
-      <c r="P19" s="159"/>
-      <c r="Q19" s="159"/>
-      <c r="R19" s="159"/>
-      <c r="S19" s="159"/>
-      <c r="T19" s="159"/>
-      <c r="U19" s="159"/>
-      <c r="V19" s="159"/>
-      <c r="W19" s="159"/>
-      <c r="X19" s="159"/>
-      <c r="Y19" s="159"/>
-      <c r="Z19" s="159"/>
-      <c r="AA19" s="159"/>
-      <c r="AB19" s="159"/>
-      <c r="AC19" s="159"/>
+      <c r="F19" s="157"/>
+      <c r="G19" s="157"/>
+      <c r="H19" s="157"/>
+      <c r="I19" s="157"/>
+      <c r="J19" s="157"/>
+      <c r="K19" s="157"/>
+      <c r="L19" s="157"/>
+      <c r="M19" s="157"/>
+      <c r="N19" s="157"/>
+      <c r="O19" s="157"/>
+      <c r="P19" s="157"/>
+      <c r="Q19" s="157"/>
+      <c r="R19" s="157"/>
+      <c r="S19" s="157"/>
+      <c r="T19" s="157"/>
+      <c r="U19" s="157"/>
+      <c r="V19" s="157"/>
+      <c r="W19" s="157"/>
+      <c r="X19" s="157"/>
+      <c r="Y19" s="157"/>
+      <c r="Z19" s="157"/>
+      <c r="AA19" s="157"/>
+      <c r="AB19" s="157"/>
+      <c r="AC19" s="157"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="K20" t="s">
@@ -5931,7 +6202,7 @@
       <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="177">
+      <c r="B23" s="5">
         <v>1.1100000000000001</v>
       </c>
       <c r="C23">
@@ -5999,11 +6270,11 @@
       </c>
       <c r="B26">
         <f>Inputs!B15</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
@@ -6212,7 +6483,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6227,7 +6498,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6242,7 +6513,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6257,7 +6528,7 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -6272,7 +6543,7 @@
         <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -6287,7 +6558,7 @@
         <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6302,7 +6573,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -6317,7 +6588,7 @@
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6375,7 +6646,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6394,23 +6665,23 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="160" t="s">
+      <c r="B1" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="F1" s="161" t="s">
+      <c r="C1" s="158"/>
+      <c r="F1" s="159" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="161"/>
-      <c r="J1" s="161" t="s">
+      <c r="G1" s="159"/>
+      <c r="J1" s="159" t="s">
         <v>119</v>
       </c>
-      <c r="K1" s="161"/>
-      <c r="N1" s="162" t="s">
+      <c r="K1" s="159"/>
+      <c r="N1" s="160" t="s">
         <v>120</v>
       </c>
-      <c r="O1" s="163"/>
-      <c r="P1" s="164"/>
+      <c r="O1" s="161"/>
+      <c r="P1" s="162"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -6999,7 +7270,7 @@
       </c>
       <c r="P18" s="60">
         <f>O18+(P5*'sub-models'!I40*'Fine Tuning'!C15)</f>
-        <v>239967.5512523081</v>
+        <v>228807.5512523081</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -7184,7 +7455,7 @@
       </c>
       <c r="P23" s="84">
         <f>SUM(P17:P22)</f>
-        <v>659348.64337047166</v>
+        <v>648188.64337047166</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -7273,7 +7544,7 @@
       </c>
       <c r="P27" s="87">
         <f>P15-P23</f>
-        <v>252238.99870427116</v>
+        <v>263398.99870427116</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -7328,7 +7599,7 @@
       </c>
       <c r="P31" s="53">
         <f>P23-P25</f>
-        <v>772968.21544015384</v>
+        <v>761808.21544015384</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -7348,7 +7619,7 @@
       </c>
       <c r="P32" s="88">
         <f>P30-P31</f>
-        <v>138619.42663458898</v>
+        <v>149779.42663458898</v>
       </c>
     </row>
     <row r="33" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7368,7 +7639,7 @@
       </c>
       <c r="P33" s="119">
         <f>P32/P30</f>
-        <v>0.15206374048588003</v>
+        <v>0.1643061179435211</v>
       </c>
     </row>
     <row r="34" spans="10:18" x14ac:dyDescent="0.25">
@@ -7407,7 +7678,7 @@
       <c r="O38" s="8"/>
       <c r="P38" s="53">
         <f>P23-O23</f>
-        <v>129881.64383561641</v>
+        <v>118721.64383561641</v>
       </c>
     </row>
     <row r="39" spans="10:18" x14ac:dyDescent="0.25">
@@ -7416,7 +7687,7 @@
       </c>
       <c r="P39" s="90">
         <f>P38/P37</f>
-        <v>14.368074232888226</v>
+        <v>13.133506331653658</v>
       </c>
     </row>
     <row r="40" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7426,7 +7697,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="120">
         <f>P39/28*1000</f>
-        <v>513.14550831743668</v>
+        <v>469.05379755905926</v>
       </c>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
@@ -7467,7 +7738,7 @@
       </c>
       <c r="P44" s="60">
         <f>P23-P25</f>
-        <v>772968.21544015384</v>
+        <v>761808.21544015384</v>
       </c>
     </row>
     <row r="45" spans="10:18" x14ac:dyDescent="0.25">
@@ -7476,11 +7747,11 @@
       </c>
       <c r="O45" s="48">
         <f>P39*P36</f>
-        <v>476713.73718924396</v>
+        <v>435752.40385591058</v>
       </c>
       <c r="P45" s="91">
         <f>P39*(P36-P37)</f>
-        <v>346832.09335362754</v>
+        <v>317030.76002029423</v>
       </c>
     </row>
     <row r="46" spans="10:18" x14ac:dyDescent="0.25">
@@ -7489,11 +7760,11 @@
       </c>
       <c r="O46" s="47">
         <f>O43-O44-O45</f>
-        <v>-208212.66671903856</v>
+        <v>-167251.33338570519</v>
       </c>
       <c r="P46" s="92">
         <f>P43-P44-P45</f>
-        <v>-208212.66671903856</v>
+        <v>-167251.33338570525</v>
       </c>
       <c r="Q46" s="6"/>
       <c r="R46" t="s">
@@ -7506,11 +7777,11 @@
       </c>
       <c r="O47" s="76">
         <f>O46/O43</f>
-        <v>-0.22840663597101155</v>
+        <v>-0.18347257648759563</v>
       </c>
       <c r="P47" s="107">
         <f>P46/P43</f>
-        <v>-0.22840663597101155</v>
+        <v>-0.18347257648759568</v>
       </c>
     </row>
     <row r="48" spans="10:18" x14ac:dyDescent="0.25">
@@ -7531,41 +7802,41 @@
     </row>
     <row r="50" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N50" s="30" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="O50">
         <f>'sub-models'!H35*Financials!O5</f>
-        <v>0</v>
+        <v>135.78</v>
       </c>
       <c r="P50" s="29">
         <f>'sub-models'!I35*Financials!P5</f>
-        <v>113.14999999999999</v>
+        <v>181.04</v>
       </c>
     </row>
     <row r="51" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N51" s="82" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="O51" s="48">
         <f>O5*'sub-models'!H39</f>
-        <v>0</v>
+        <v>67890</v>
       </c>
       <c r="P51" s="91">
         <f>P5*'sub-models'!I39</f>
-        <v>90520</v>
+        <v>144832</v>
       </c>
     </row>
     <row r="52" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N52" s="30" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="O52" s="75">
         <f>'sub-models'!H48</f>
-        <v>1</v>
+        <v>0.92486377396569119</v>
       </c>
       <c r="P52" s="94">
         <f>'sub-models'!I48</f>
-        <v>0.93738647830474264</v>
+        <v>0.89981836528758841</v>
       </c>
     </row>
     <row r="53" spans="14:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7575,7 +7846,7 @@
       <c r="O53" s="10"/>
       <c r="P53" s="107">
         <f>O52-P52</f>
-        <v>6.2613521695257357E-2</v>
+        <v>2.5045408678102787E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7592,10 +7863,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E517695-1630-4E1E-9003-CFDB8A26EAE4}">
-  <dimension ref="A2:AQ60"/>
+  <dimension ref="A2:AU60"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7603,7 +7874,7 @@
     <col min="1" max="1" width="14" style="68" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="68"/>
+    <col min="6" max="6" width="42.85546875" style="68" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
     <col min="9" max="9" width="17.140625" customWidth="1"/>
@@ -7631,22 +7902,23 @@
     <col min="36" max="36" width="10.7109375" customWidth="1"/>
     <col min="38" max="38" width="8.7109375" style="68"/>
     <col min="39" max="39" width="40.140625" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="68"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="169" t="s">
+      <c r="C2" s="167" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="169"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="100" t="s">
         <v>171</v>
       </c>
       <c r="F2" s="66"/>
     </row>
-    <row r="3" spans="1:43" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66"/>
       <c r="F3" s="66"/>
       <c r="K3" s="66"/>
@@ -7655,8 +7927,9 @@
       <c r="Y3" s="66"/>
       <c r="AC3" s="66"/>
       <c r="AL3" s="66"/>
-    </row>
-    <row r="4" spans="1:43" s="32" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="AS3" s="66"/>
+    </row>
+    <row r="4" spans="1:47" s="32" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="67"/>
       <c r="B4" s="32" t="s">
         <v>172</v>
@@ -7686,19 +7959,23 @@
         <v>178</v>
       </c>
       <c r="AL4" s="67"/>
-      <c r="AM4" s="160" t="s">
-        <v>372</v>
-      </c>
-      <c r="AN4" s="160"/>
-      <c r="AO4" s="160"/>
-      <c r="AP4" s="160"/>
-      <c r="AQ4" s="160"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B5" s="170" t="s">
+      <c r="AM4" s="158" t="s">
+        <v>368</v>
+      </c>
+      <c r="AN4" s="158"/>
+      <c r="AO4" s="158"/>
+      <c r="AP4" s="158"/>
+      <c r="AQ4" s="158"/>
+      <c r="AS4" s="67"/>
+      <c r="AU4" s="32" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="B5" s="168" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="169"/>
       <c r="G5" t="s">
         <v>180</v>
       </c>
@@ -7709,7 +7986,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
         <v>183</v>
       </c>
@@ -7732,8 +8009,11 @@
       <c r="W6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AU6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="Q7" s="27" t="s">
         <v>189</v>
       </c>
@@ -7743,19 +8023,22 @@
       <c r="W7" t="s">
         <v>188</v>
       </c>
-      <c r="AD7" s="165" t="s">
+      <c r="AD7" s="163" t="s">
         <v>191</v>
       </c>
-      <c r="AE7" s="166"/>
-      <c r="AF7" s="166"/>
-      <c r="AG7" s="166"/>
-      <c r="AH7" s="166"/>
-      <c r="AI7" s="167"/>
+      <c r="AE7" s="164"/>
+      <c r="AF7" s="164"/>
+      <c r="AG7" s="164"/>
+      <c r="AH7" s="164"/>
+      <c r="AI7" s="165"/>
       <c r="AM7" s="137" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="Q8" t="s">
         <v>192</v>
       </c>
@@ -7785,10 +8068,13 @@
         <v>199</v>
       </c>
       <c r="AM8" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="V9" t="s">
         <v>200</v>
       </c>
@@ -7816,17 +8102,20 @@
         <v>310</v>
       </c>
       <c r="AM9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
-        <v>395</v>
-      </c>
-      <c r="G10" s="173"/>
-      <c r="H10" s="173"/>
-      <c r="I10" s="173"/>
-      <c r="J10" s="173"/>
+        <v>391</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
       <c r="L10" s="4" t="s">
         <v>202</v>
       </c>
@@ -7892,17 +8181,18 @@
         <v>15</v>
       </c>
       <c r="AM10" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>210</v>
       </c>
-      <c r="G11" s="172"/>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="172"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
       <c r="L11" t="s">
         <v>211</v>
       </c>
@@ -7959,20 +8249,21 @@
         <v>300</v>
       </c>
       <c r="AM11" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>215</v>
       </c>
       <c r="C12" t="s">
         <v>216</v>
       </c>
-      <c r="G12" s="172"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="172"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
       <c r="L12" t="s">
         <v>217</v>
       </c>
@@ -8017,18 +8308,20 @@
         <f>$X$23</f>
         <v>2.1600000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AU12" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>221</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="G13" s="172"/>
-      <c r="H13" s="172"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="172"/>
+      <c r="G13" s="4" t="s">
+        <v>403</v>
+      </c>
       <c r="L13" t="s">
         <v>223</v>
       </c>
@@ -8081,12 +8374,16 @@
         <f t="shared" si="0"/>
         <v>30132</v>
       </c>
-    </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="G14" s="172"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="172"/>
+      <c r="AU13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="G14" s="170" t="s">
+        <v>404</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="Q14" t="s">
         <v>227</v>
       </c>
@@ -8102,7 +8399,7 @@
         <v>228</v>
       </c>
       <c r="AM14" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AN14">
         <v>55</v>
@@ -8112,7 +8409,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>202</v>
       </c>
@@ -8125,10 +8422,7 @@
       <c r="E15" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="G15" s="172"/>
-      <c r="H15" s="178"/>
-      <c r="I15" s="172"/>
-      <c r="J15" s="172"/>
+      <c r="H15" s="3"/>
       <c r="L15" t="s">
         <v>229</v>
       </c>
@@ -8143,16 +8437,16 @@
         <f>S14*S16</f>
         <v>10573.333333333334</v>
       </c>
-      <c r="AD15" s="165" t="s">
+      <c r="AD15" s="163" t="s">
         <v>231</v>
       </c>
-      <c r="AE15" s="166"/>
-      <c r="AF15" s="166"/>
-      <c r="AG15" s="166"/>
-      <c r="AH15" s="166"/>
-      <c r="AI15" s="167"/>
+      <c r="AE15" s="164"/>
+      <c r="AF15" s="164"/>
+      <c r="AG15" s="164"/>
+      <c r="AH15" s="164"/>
+      <c r="AI15" s="165"/>
       <c r="AM15" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AN15" s="26">
         <f>'Fine Tuning'!B37</f>
@@ -8163,10 +8457,10 @@
         <v>0.85</v>
       </c>
       <c r="AP15" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>232</v>
       </c>
@@ -8178,10 +8472,11 @@
         <f>C16</f>
         <v>1.6</v>
       </c>
-      <c r="G16" s="172"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="172"/>
+      <c r="G16" t="s">
+        <v>412</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="152"/>
       <c r="L16" s="4" t="s">
         <v>233</v>
       </c>
@@ -8220,7 +8515,7 @@
         <v>199</v>
       </c>
       <c r="AM16" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="AN16">
         <f>IF((VLOOKUP('Fine Tuning'!B15,'Fine Tuning'!N2:P8,3,))&gt;Inputs!B17,Inputs!B17,(VLOOKUP('Fine Tuning'!B15,'Fine Tuning'!N2:P8,3,)))</f>
@@ -8238,10 +8533,9 @@
         <f>C17</f>
         <v>11.5</v>
       </c>
-      <c r="G17" s="172"/>
-      <c r="H17" s="172"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="172"/>
+      <c r="G17" t="s">
+        <v>413</v>
+      </c>
       <c r="Q17" t="s">
         <v>238</v>
       </c>
@@ -8276,7 +8570,7 @@
         <v>21092.399999999998</v>
       </c>
       <c r="AN17" s="4" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -8291,10 +8585,9 @@
         <f>C18/100</f>
         <v>0.01</v>
       </c>
-      <c r="G18" s="181"/>
-      <c r="H18" s="182"/>
-      <c r="I18" s="182"/>
-      <c r="J18" s="182"/>
+      <c r="G18" s="170" t="s">
+        <v>414</v>
+      </c>
       <c r="L18" t="s">
         <v>241</v>
       </c>
@@ -8322,16 +8615,16 @@
         <v>1066.338</v>
       </c>
       <c r="AI18" s="60">
-        <f t="shared" si="2"/>
+        <f>AI17/2</f>
         <v>10546.199999999999</v>
       </c>
       <c r="AJ18" s="57"/>
       <c r="AM18" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AN18" s="3">
         <f>(Inputs!B15-Inputs!B10)*AN16</f>
-        <v>300</v>
+        <v>120.00000000000004</v>
       </c>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.25">
@@ -8342,10 +8635,6 @@
         <f>D18*D16*D17</f>
         <v>0.184</v>
       </c>
-      <c r="G19" s="182"/>
-      <c r="H19" s="182"/>
-      <c r="I19" s="182"/>
-      <c r="J19" s="182"/>
       <c r="L19" s="4" t="s">
         <v>243</v>
       </c>
@@ -8400,10 +8689,9 @@
         <f>E19*'Fine Tuning'!B5/'Fine Tuning'!B3</f>
         <v>72.116129032258058</v>
       </c>
-      <c r="G20" s="182"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182"/>
+      <c r="G20" t="s">
+        <v>437</v>
+      </c>
       <c r="Q20" s="4" t="s">
         <v>247</v>
       </c>
@@ -8440,18 +8728,14 @@
         <v>10546.199999999999</v>
       </c>
       <c r="AM20" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AN20">
         <f>AO15*AN18</f>
-        <v>255</v>
+        <v>102.00000000000003</v>
       </c>
     </row>
     <row r="21" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="G21" s="182"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="182"/>
-      <c r="J21" s="182"/>
       <c r="L21" t="s">
         <v>249</v>
       </c>
@@ -8463,30 +8747,36 @@
       <c r="B22" t="s">
         <v>251</v>
       </c>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
-      <c r="J22" s="181"/>
-      <c r="AD22" s="165" t="s">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="AD22" s="163" t="s">
         <v>252</v>
       </c>
-      <c r="AE22" s="166"/>
-      <c r="AF22" s="166"/>
-      <c r="AG22" s="166"/>
-      <c r="AH22" s="166"/>
-      <c r="AI22" s="167"/>
+      <c r="AE22" s="164"/>
+      <c r="AF22" s="164"/>
+      <c r="AG22" s="164"/>
+      <c r="AH22" s="164"/>
+      <c r="AI22" s="165"/>
       <c r="AM22" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="AN22">
         <f>AN20*AN14</f>
-        <v>14025</v>
+        <v>5610.0000000000018</v>
       </c>
     </row>
     <row r="23" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>253</v>
       </c>
+      <c r="L23" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>403</v>
+      </c>
       <c r="V23" t="s">
         <v>254</v>
       </c>
@@ -8516,21 +8806,21 @@
         <v>199</v>
       </c>
       <c r="AM23" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AN23">
         <f>AO14*AN20</f>
-        <v>14.025</v>
+        <v>5.6100000000000012</v>
       </c>
     </row>
     <row r="24" spans="2:40" x14ac:dyDescent="0.25">
       <c r="G24" s="139" t="s">
-        <v>355</v>
-      </c>
-      <c r="H24" s="139" t="s">
+        <v>351</v>
+      </c>
+      <c r="H24" s="171" t="s">
         <v>121</v>
       </c>
-      <c r="I24" s="139" t="s">
+      <c r="I24" s="171" t="s">
         <v>122</v>
       </c>
       <c r="V24" t="s">
@@ -8548,7 +8838,7 @@
         <v>0</v>
       </c>
       <c r="AG24" s="6">
-        <f t="shared" si="4"/>
+        <f>AG13-AG17</f>
         <v>0</v>
       </c>
       <c r="AH24" s="6">
@@ -8562,16 +8852,16 @@
     </row>
     <row r="25" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G25" s="124" t="s">
-        <v>337</v>
-      </c>
-      <c r="H25" s="140">
+        <v>406</v>
+      </c>
+      <c r="H25" s="172">
         <f>'Fine Tuning'!B11</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="140">
+        <v>1.2</v>
+      </c>
+      <c r="I25" s="172">
         <f>IF(H25-I27&gt;0,H25-I27,0)</f>
         <v>0</v>
       </c>
@@ -8579,6 +8869,12 @@
         <f>IF((I25-J27)&lt;0,(I25-J25),0)</f>
         <v>0</v>
       </c>
+      <c r="L25" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>419</v>
+      </c>
       <c r="V25" s="27" t="s">
         <v>256</v>
       </c>
@@ -8612,7 +8908,7 @@
         <v>4519.8</v>
       </c>
       <c r="AM25" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="AN25" s="3">
         <f>Inputs!B5</f>
@@ -8624,15 +8920,18 @@
         <v>258</v>
       </c>
       <c r="G26" s="125" t="s">
-        <v>339</v>
-      </c>
-      <c r="H26" s="141">
+        <v>337</v>
+      </c>
+      <c r="H26" s="173">
         <f>'Fine Tuning'!B12</f>
         <v>500</v>
       </c>
-      <c r="I26" s="141">
+      <c r="I26" s="173">
         <f>H26</f>
         <v>500</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>420</v>
       </c>
       <c r="V26" t="s">
         <v>259</v>
@@ -8666,7 +8965,7 @@
       </c>
       <c r="AJ26" s="6"/>
       <c r="AM26" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AN26">
         <f>Inputs!B3</f>
@@ -8678,15 +8977,18 @@
         <v>260</v>
       </c>
       <c r="G27" s="124" t="s">
-        <v>338</v>
-      </c>
-      <c r="H27" s="124" t="str">
+        <v>405</v>
+      </c>
+      <c r="H27" s="174" t="str">
         <f>"- "</f>
         <v xml:space="preserve">- </v>
       </c>
-      <c r="I27" s="124">
+      <c r="I27" s="174">
         <f>'Fine Tuning'!B26</f>
-        <v>1</v>
+        <v>1.6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>434</v>
       </c>
       <c r="AD27" s="50" t="s">
         <v>44</v>
@@ -8717,15 +9019,18 @@
         <v>261</v>
       </c>
       <c r="G28" s="125" t="s">
-        <v>340</v>
-      </c>
-      <c r="H28" s="125" t="str">
+        <v>338</v>
+      </c>
+      <c r="H28" s="175" t="str">
         <f>"- "</f>
         <v xml:space="preserve">- </v>
       </c>
-      <c r="I28" s="141">
+      <c r="I28" s="173">
         <f>'Fine Tuning'!B27</f>
         <v>800</v>
+      </c>
+      <c r="L28" t="s">
+        <v>418</v>
       </c>
       <c r="V28" s="4" t="s">
         <v>262</v>
@@ -8735,11 +9040,11 @@
         <v>101.95200000000001</v>
       </c>
       <c r="AM28" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="AN28" s="47">
         <f>AN23*AN26</f>
-        <v>4347.75</v>
+        <v>1739.1000000000004</v>
       </c>
     </row>
     <row r="29" spans="2:40" x14ac:dyDescent="0.25">
@@ -8750,34 +9055,37 @@
         <v>226</v>
       </c>
       <c r="G29" s="124" t="s">
-        <v>341</v>
-      </c>
-      <c r="H29" s="124"/>
-      <c r="I29" s="140">
+        <v>339</v>
+      </c>
+      <c r="H29" s="174"/>
+      <c r="I29" s="172">
         <f>SUM(I25+I27)-H25</f>
-        <v>1</v>
+        <v>0.40000000000000013</v>
+      </c>
+      <c r="L29" t="s">
+        <v>416</v>
       </c>
       <c r="V29" t="s">
         <v>264</v>
       </c>
       <c r="W29">
-        <f>W23*W26</f>
-        <v>101.952</v>
-      </c>
-      <c r="AD29" s="165" t="s">
+        <f>W23*W26/1000</f>
+        <v>0.101952</v>
+      </c>
+      <c r="AD29" s="163" t="s">
         <v>265</v>
       </c>
-      <c r="AE29" s="166"/>
-      <c r="AF29" s="166"/>
-      <c r="AG29" s="168"/>
+      <c r="AE29" s="164"/>
+      <c r="AF29" s="164"/>
+      <c r="AG29" s="166"/>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="AM29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AN29" s="47">
         <f>AN28*AN25</f>
-        <v>30434.25</v>
+        <v>12173.700000000003</v>
       </c>
     </row>
     <row r="30" spans="2:40" x14ac:dyDescent="0.25">
@@ -8792,12 +9100,15 @@
         <v>267</v>
       </c>
       <c r="G30" s="125" t="s">
-        <v>342</v>
-      </c>
-      <c r="H30" s="125"/>
-      <c r="I30" s="141">
+        <v>340</v>
+      </c>
+      <c r="H30" s="175"/>
+      <c r="I30" s="173">
         <f>IF(H25=0,I28,I28-I26)</f>
-        <v>800</v>
+        <v>300</v>
+      </c>
+      <c r="L30" t="s">
+        <v>417</v>
       </c>
       <c r="AD30" s="52" t="s">
         <v>236</v>
@@ -8821,8 +9132,8 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="G31" s="124"/>
-      <c r="H31" s="124"/>
-      <c r="I31" s="124"/>
+      <c r="H31" s="174"/>
+      <c r="I31" s="174"/>
       <c r="V31" t="s">
         <v>273</v>
       </c>
@@ -8849,32 +9160,32 @@
       <c r="B32" t="s">
         <v>274</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="25">
         <f>C30*C31</f>
         <v>5.5500000000000007</v>
       </c>
-      <c r="G32" s="142" t="s">
-        <v>343</v>
-      </c>
-      <c r="H32" s="124"/>
-      <c r="I32" s="124"/>
+      <c r="G32" s="140" t="s">
+        <v>341</v>
+      </c>
+      <c r="H32" s="174"/>
+      <c r="I32" s="174"/>
       <c r="AD32" s="56" t="s">
         <v>38</v>
       </c>
       <c r="AE32" s="6">
-        <f t="shared" ref="AE32:AE34" si="7">SUM($AE$13:$AI$13)</f>
+        <f>SUM($AE$13:$AI$13)</f>
         <v>33178.68</v>
       </c>
       <c r="AF32" s="6">
-        <f t="shared" ref="AF32:AF34" si="8">SUM(AE25:AI25)</f>
+        <f t="shared" ref="AF32:AF34" si="7">SUM(AE25:AI25)</f>
         <v>4976.8020000000006</v>
       </c>
       <c r="AG32" s="64">
-        <f t="shared" ref="AG32:AG34" si="9">AF32/AE32</f>
+        <f t="shared" ref="AG32:AG34" si="8">AF32/AE32</f>
         <v>0.15000000000000002</v>
       </c>
     </row>
-    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>276</v>
       </c>
@@ -8885,33 +9196,39 @@
         <v>277</v>
       </c>
       <c r="G33" s="124" t="s">
-        <v>344</v>
-      </c>
-      <c r="H33" s="124">
+        <v>407</v>
+      </c>
+      <c r="H33" s="174">
         <f>H25*365/1000</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="124">
+        <v>0.438</v>
+      </c>
+      <c r="I33" s="174">
         <f>I25*365/1000</f>
         <v>0</v>
       </c>
+      <c r="L33" t="s">
+        <v>435</v>
+      </c>
+      <c r="V33" t="s">
+        <v>403</v>
+      </c>
       <c r="AD33" s="56" t="s">
         <v>41</v>
       </c>
       <c r="AE33" s="6">
+        <f t="shared" ref="AE32:AE34" si="9">SUM($AE$13:$AI$13)</f>
+        <v>33178.68</v>
+      </c>
+      <c r="AF33" s="6">
         <f t="shared" si="7"/>
-        <v>33178.68</v>
-      </c>
-      <c r="AF33" s="6">
+        <v>9039.6</v>
+      </c>
+      <c r="AG33" s="64">
         <f t="shared" si="8"/>
-        <v>9039.6</v>
-      </c>
-      <c r="AG33" s="64">
-        <f t="shared" si="9"/>
         <v>0.27245206861755805</v>
       </c>
     </row>
-    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>279</v>
       </c>
@@ -8923,33 +9240,36 @@
         <v>280</v>
       </c>
       <c r="G34" s="125" t="s">
-        <v>345</v>
-      </c>
-      <c r="H34" s="125" t="str">
+        <v>408</v>
+      </c>
+      <c r="H34" s="175" t="str">
         <f>"- "</f>
         <v xml:space="preserve">- </v>
       </c>
-      <c r="I34" s="125">
+      <c r="I34" s="175">
         <f>I27*365/1000</f>
-        <v>0.36499999999999999</v>
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="V34" t="s">
+        <v>421</v>
       </c>
       <c r="AD34" s="50" t="s">
         <v>44</v>
       </c>
       <c r="AE34" s="38">
+        <f t="shared" si="9"/>
+        <v>33178.68</v>
+      </c>
+      <c r="AF34" s="38">
         <f t="shared" si="7"/>
-        <v>33178.68</v>
-      </c>
-      <c r="AF34" s="38">
+        <v>4519.8</v>
+      </c>
+      <c r="AG34" s="65">
         <f t="shared" si="8"/>
-        <v>4519.8</v>
-      </c>
-      <c r="AG34" s="65">
-        <f t="shared" si="9"/>
         <v>0.13622603430877903</v>
       </c>
     </row>
-    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>282</v>
       </c>
@@ -8958,18 +9278,18 @@
         <v>4720</v>
       </c>
       <c r="G35" s="124" t="s">
-        <v>350</v>
-      </c>
-      <c r="H35" s="124">
+        <v>346</v>
+      </c>
+      <c r="H35" s="174">
         <f>H33</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="124">
+        <v>0.438</v>
+      </c>
+      <c r="I35" s="174">
         <f>I33+I34</f>
-        <v>0.36499999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>284</v>
       </c>
@@ -8977,13 +9297,13 @@
         <f>C35*C33</f>
         <v>23.6</v>
       </c>
-      <c r="G36" s="142" t="s">
-        <v>346</v>
-      </c>
-      <c r="H36" s="124"/>
-      <c r="I36" s="124"/>
-    </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="G36" s="140" t="s">
+        <v>342</v>
+      </c>
+      <c r="H36" s="174"/>
+      <c r="I36" s="174"/>
+    </row>
+    <row r="37" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>286</v>
       </c>
@@ -8992,54 +9312,98 @@
         <v>130.98000000000002</v>
       </c>
       <c r="G37" s="124" t="s">
-        <v>347</v>
-      </c>
-      <c r="H37" s="143">
+        <v>343</v>
+      </c>
+      <c r="H37" s="177">
         <f>H33*H26</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="144">
+        <v>219</v>
+      </c>
+      <c r="I37" s="176">
         <f>I33*I26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:39" x14ac:dyDescent="0.25">
       <c r="G38" s="125" t="s">
-        <v>348</v>
-      </c>
-      <c r="H38" s="125"/>
-      <c r="I38" s="141">
+        <v>344</v>
+      </c>
+      <c r="H38" s="175"/>
+      <c r="I38" s="173">
         <f>I34*I28</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
+        <v>467.2</v>
+      </c>
+      <c r="AD38" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="AM38" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="39" spans="2:39" x14ac:dyDescent="0.25">
       <c r="G39" s="124" t="s">
-        <v>351</v>
-      </c>
-      <c r="H39" s="143">
+        <v>347</v>
+      </c>
+      <c r="H39" s="177">
         <f>SUM(H37:H38)</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="143">
+        <v>219</v>
+      </c>
+      <c r="I39" s="177">
         <f>SUM(I37:I38)</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
+        <v>467.2</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="40" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>397</v>
+      </c>
       <c r="G40" s="124" t="s">
-        <v>349</v>
-      </c>
-      <c r="H40" s="124" t="str">
+        <v>345</v>
+      </c>
+      <c r="H40" s="175" t="str">
         <f>" - "</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="I40" s="143">
+      <c r="I40" s="178">
         <f>I39-H39</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
+        <v>248.2</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>426</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="41" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>398</v>
+      </c>
+      <c r="C41" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>427</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="42" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>399</v>
+      </c>
+      <c r="C42" t="s">
+        <v>409</v>
+      </c>
+      <c r="AD42">
+        <f>310*15*300*0.0216*0.3*1</f>
+        <v>9039.6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:39" x14ac:dyDescent="0.25">
       <c r="G43" s="4" t="s">
         <v>268</v>
       </c>
@@ -9049,44 +9413,71 @@
       <c r="I43" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AM43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>400</v>
+      </c>
+      <c r="C44" t="s">
+        <v>411</v>
+      </c>
       <c r="G44" t="s">
         <v>272</v>
       </c>
       <c r="H44" s="3">
         <f>H25*365</f>
-        <v>0</v>
+        <v>438</v>
       </c>
       <c r="I44" s="3">
         <f>I25*365</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="AD44" t="s">
+        <v>423</v>
+      </c>
+      <c r="AM44" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="45" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>402</v>
+      </c>
+      <c r="C45" t="s">
+        <v>401</v>
+      </c>
       <c r="G45" s="8" t="s">
         <v>275</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9">
         <f>I27*365</f>
-        <v>365</v>
-      </c>
-    </row>
-    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="46" spans="2:39" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>278</v>
       </c>
       <c r="H46" s="3">
         <f>SUM(H44:H45)</f>
-        <v>0</v>
+        <v>438</v>
       </c>
       <c r="I46" s="3">
         <f>SUM(I44:I45)</f>
-        <v>365</v>
-      </c>
-    </row>
-    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="47" spans="2:39" x14ac:dyDescent="0.25">
       <c r="G47" s="8" t="s">
         <v>281</v>
       </c>
@@ -9099,17 +9490,17 @@
         <v>4955</v>
       </c>
     </row>
-    <row r="48" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G48" s="73" t="s">
         <v>283</v>
       </c>
       <c r="H48" s="74">
         <f>(H47-(H46*I49))/H47</f>
-        <v>1</v>
+        <v>0.92486377396569119</v>
       </c>
       <c r="I48" s="74">
         <f>(I47-(I46*I49))/I47</f>
-        <v>0.93738647830474264</v>
+        <v>0.89981836528758841</v>
       </c>
     </row>
     <row r="49" spans="7:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -11016,28 +11407,28 @@
       <c r="I44"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="161" t="s">
+      <c r="A45" s="159" t="s">
         <v>330</v>
       </c>
-      <c r="B45" s="161"/>
-      <c r="C45" s="161"/>
-      <c r="D45" s="161"/>
-      <c r="E45" s="161"/>
-      <c r="F45" s="161"/>
-      <c r="G45" s="161"/>
-      <c r="H45" s="161"/>
-      <c r="I45" s="161"/>
+      <c r="B45" s="159"/>
+      <c r="C45" s="159"/>
+      <c r="D45" s="159"/>
+      <c r="E45" s="159"/>
+      <c r="F45" s="159"/>
+      <c r="G45" s="159"/>
+      <c r="H45" s="159"/>
+      <c r="I45" s="159"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="161"/>
-      <c r="B46" s="161"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="161"/>
-      <c r="E46" s="161"/>
-      <c r="F46" s="161"/>
-      <c r="G46" s="161"/>
-      <c r="H46" s="161"/>
-      <c r="I46" s="161"/>
+      <c r="A46" s="159"/>
+      <c r="B46" s="159"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="159"/>
+      <c r="E46" s="159"/>
+      <c r="F46" s="159"/>
+      <c r="G46" s="159"/>
+      <c r="H46" s="159"/>
+      <c r="I46" s="159"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">

</xml_diff>